<commit_message>
Re-assigned pins to be able to make one loom to the charge port and one to the car
</commit_message>
<xml_diff>
--- a/pcb/production/qca7000_2024-04-05/FOCCI-BOM_JLCSMT.xlsx
+++ b/pcb/production/qca7000_2024-04-05/FOCCI-BOM_JLCSMT.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="191">
   <si>
     <t xml:space="preserve">Comment</t>
   </si>
@@ -420,6 +420,7 @@
         <color rgb="FF000000"/>
         <rFont val="宋体"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">, R52, R64</t>
     </r>
@@ -609,6 +610,9 @@
   </si>
   <si>
     <t xml:space="preserve">Package_DFN_QFN:QFN-68-1EP_8x8mm_P0.4mm_EP5.2x5.2mm_ThermalVias</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C9900078626</t>
   </si>
   <si>
     <t xml:space="preserve">25MHz</t>
@@ -710,6 +714,7 @@
       <color rgb="FF000000"/>
       <name val="宋体"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1045,8 +1050,8 @@
   </sheetPr>
   <dimension ref="A1:D1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B36" activeCellId="0" sqref="B36"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D56" activeCellId="0" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="20" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1823,47 +1828,50 @@
       <c r="C55" s="2" t="s">
         <v>177</v>
       </c>
+      <c r="D55" s="2" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="56" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D58" s="7" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>